<commit_message>
Re-add monthly data files
</commit_message>
<xml_diff>
--- a/EV Yearly sales.xlsx
+++ b/EV Yearly sales.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anu\Documents\Project1 data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spenser Hilton\Desktop\BootcampProj1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -193,6 +193,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> http://hybridcars.com</t>
     </r>
@@ -223,6 +224,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> text are estimated values.
 Values in </t>
@@ -240,6 +242,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> text do not distinguish the difference between PEVs and PHEVs.</t>
     </r>
@@ -406,6 +409,7 @@
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -428,6 +432,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -885,7 +890,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -909,27 +914,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -954,6 +938,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="26" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="163">
     <cellStyle name="20% - Accent1 2" xfId="1"/>
@@ -1526,7 +1532,7 @@
   <dimension ref="A1:BD40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1538,977 +1544,1013 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="25">
+      <c r="C1" s="18">
         <v>2011</v>
       </c>
-      <c r="D1" s="25">
+      <c r="D1" s="18">
         <v>2012</v>
       </c>
-      <c r="E1" s="25">
+      <c r="E1" s="18">
         <v>2013</v>
       </c>
-      <c r="F1" s="25">
+      <c r="F1" s="18">
         <v>2014</v>
       </c>
-      <c r="G1" s="25">
+      <c r="G1" s="18">
         <v>2015</v>
       </c>
-      <c r="H1" s="25">
+      <c r="H1" s="18">
         <v>2016</v>
       </c>
-      <c r="I1" s="25">
+      <c r="I1" s="18">
         <v>2017</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="22">
         <v>9674</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="22">
         <v>9819</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="22">
         <v>22610</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="22">
         <v>30200</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="22">
         <v>17269</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="23">
         <v>14006</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="23">
         <v>11230</v>
       </c>
-      <c r="J2" s="31">
-        <v>103578</v>
+      <c r="J2" s="24">
+        <f>SUM(C2:I2)</f>
+        <v>114808</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="22">
         <v>7671</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="22">
         <v>23461</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="22">
         <v>23094</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="22">
         <v>18805</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="22">
         <v>15393</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="23">
         <v>24739</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="23">
         <v>20349</v>
       </c>
-      <c r="J3" s="31">
-        <v>113163</v>
+      <c r="J3" s="24">
+        <f t="shared" ref="J3:J29" si="0">SUM(C3:I3)</f>
+        <v>133512</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="29">
-        <v>0</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+      <c r="D4" s="22">
         <v>2171</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="22">
         <v>19000</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="22">
         <v>16750</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="22">
         <v>26200</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="23">
         <v>29156</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="23">
         <v>27060</v>
       </c>
-      <c r="J4" s="31">
-        <v>93277</v>
+      <c r="J4" s="24">
+        <f t="shared" si="0"/>
+        <v>120337</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="33">
-        <v>0</v>
-      </c>
-      <c r="D5" s="33">
+      <c r="C5" s="26">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26">
         <v>12749</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="26">
         <v>12088</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="26">
         <v>13264</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="26">
         <v>4191</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="27">
         <v>2474</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="27">
         <v>20936</v>
       </c>
-      <c r="J5" s="31">
-        <v>44766</v>
+      <c r="J5" s="24">
+        <f t="shared" si="0"/>
+        <v>65702</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="29">
-        <v>0</v>
-      </c>
-      <c r="D6" s="29">
-        <v>0</v>
-      </c>
-      <c r="E6" s="29">
+      <c r="C6" s="22">
+        <v>0</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
         <v>6089</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="22">
         <v>11550</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="22">
         <v>9750</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="23">
         <v>15938</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="23">
         <v>9632</v>
       </c>
-      <c r="J6" s="31">
-        <v>43327</v>
+      <c r="J6" s="24">
+        <f t="shared" si="0"/>
+        <v>52959</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="29">
-        <v>0</v>
-      </c>
-      <c r="D7" s="29">
+      <c r="C7" s="22">
+        <v>0</v>
+      </c>
+      <c r="D7" s="22">
         <v>2374</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="22">
         <v>7154</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="22">
         <v>8433</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="22">
         <v>7591</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="23">
         <v>7957</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="23">
         <v>8140</v>
       </c>
-      <c r="J7" s="31">
-        <v>33509</v>
+      <c r="J7" s="24">
+        <f t="shared" si="0"/>
+        <v>41649</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="29">
-        <v>0</v>
-      </c>
-      <c r="D8" s="29">
-        <v>0</v>
-      </c>
-      <c r="E8" s="29">
-        <v>0</v>
-      </c>
-      <c r="F8" s="29">
+      <c r="C8" s="22">
+        <v>0</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
         <v>6092</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="22">
         <v>11004</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="28">
         <v>7625</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="28">
         <v>6276</v>
       </c>
-      <c r="J8" s="31">
-        <v>24721</v>
+      <c r="J8" s="24">
+        <f t="shared" si="0"/>
+        <v>30997</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="29">
-        <v>0</v>
-      </c>
-      <c r="D9" s="29">
+      <c r="C9" s="22">
+        <v>0</v>
+      </c>
+      <c r="D9" s="22">
         <v>683</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="22">
         <v>1738</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="22">
         <v>1964</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="22">
         <v>1582</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="23">
         <v>872</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="23">
         <v>1817</v>
       </c>
-      <c r="J9" s="31">
-        <v>6839</v>
+      <c r="J9" s="24">
+        <f t="shared" si="0"/>
+        <v>8656</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="29">
-        <v>0</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0</v>
-      </c>
-      <c r="E10" s="29">
+      <c r="C10" s="22">
+        <v>0</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0</v>
+      </c>
+      <c r="E10" s="22">
         <v>260</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="22">
         <v>1503</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="22">
         <v>4569</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="23">
         <v>3897</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="23">
         <v>5380</v>
       </c>
-      <c r="J10" s="31">
-        <v>10229</v>
+      <c r="J10" s="24">
+        <f t="shared" si="0"/>
+        <v>15609</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="29">
-        <v>0</v>
-      </c>
-      <c r="D11" s="29">
+      <c r="C11" s="22">
+        <v>0</v>
+      </c>
+      <c r="D11" s="22">
         <v>137</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="22">
         <v>923</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="22">
         <v>2594</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="22">
         <v>1387</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="23">
         <v>657</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="23">
         <v>544</v>
       </c>
-      <c r="J11" s="31">
-        <v>5698</v>
+      <c r="J11" s="24">
+        <f t="shared" si="0"/>
+        <v>6242</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="29">
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0</v>
-      </c>
-      <c r="E12" s="29">
-        <v>0</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="C12" s="22">
+        <v>0</v>
+      </c>
+      <c r="D12" s="22">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
         <v>357</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="22">
         <v>4232</v>
       </c>
-      <c r="H12" s="36">
-        <v>0</v>
-      </c>
-      <c r="I12" s="36">
+      <c r="H12" s="29">
+        <v>0</v>
+      </c>
+      <c r="I12" s="29">
         <v>3534</v>
       </c>
-      <c r="J12" s="31">
-        <v>4589</v>
+      <c r="J12" s="24">
+        <f t="shared" si="0"/>
+        <v>8123</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="29">
-        <v>0</v>
-      </c>
-      <c r="D13" s="29">
-        <v>0</v>
-      </c>
-      <c r="E13" s="29">
+      <c r="C13" s="22">
+        <v>0</v>
+      </c>
+      <c r="D13" s="22">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22">
         <v>560</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="22">
         <v>1145</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="22">
         <v>2629</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="23">
         <v>3035</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="23">
         <v>23</v>
       </c>
-      <c r="J13" s="31">
-        <v>7369</v>
+      <c r="J13" s="24">
+        <f t="shared" si="0"/>
+        <v>7392</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="29">
-        <v>0</v>
-      </c>
-      <c r="D14" s="29">
-        <v>0</v>
-      </c>
-      <c r="E14" s="29">
-        <v>0</v>
-      </c>
-      <c r="F14" s="29">
+      <c r="C14" s="22">
+        <v>0</v>
+      </c>
+      <c r="D14" s="22">
+        <v>0</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0</v>
+      </c>
+      <c r="F14" s="22">
         <v>555</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="22">
         <v>2265</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="23">
         <v>1594</v>
       </c>
-      <c r="I14" s="30">
+      <c r="I14" s="23">
         <v>488</v>
       </c>
-      <c r="J14" s="31">
-        <v>4414</v>
+      <c r="J14" s="24">
+        <f t="shared" si="0"/>
+        <v>4902</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="29">
-        <v>0</v>
-      </c>
-      <c r="D15" s="29">
-        <v>0</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0</v>
-      </c>
-      <c r="F15" s="29">
+      <c r="C15" s="22">
+        <v>0</v>
+      </c>
+      <c r="D15" s="22">
+        <v>0</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0</v>
+      </c>
+      <c r="F15" s="22">
         <v>774</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="22">
         <v>1906</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="23">
         <v>632</v>
       </c>
-      <c r="I15" s="30">
+      <c r="I15" s="23">
         <v>744</v>
       </c>
-      <c r="J15" s="31">
-        <v>3312</v>
+      <c r="J15" s="24">
+        <f t="shared" si="0"/>
+        <v>4056</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="29">
-        <v>0</v>
-      </c>
-      <c r="D16" s="29">
+      <c r="C16" s="22">
+        <v>0</v>
+      </c>
+      <c r="D16" s="22">
         <v>192</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="22">
         <v>1005</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="22">
         <v>1184</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="22">
         <v>18</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="24">
+        <f t="shared" si="0"/>
         <v>2399</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="29">
-        <v>0</v>
-      </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="29">
+      <c r="C17" s="22">
+        <v>0</v>
+      </c>
+      <c r="D17" s="22">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22">
         <v>6</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="22">
         <v>1310</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="22">
         <v>1024</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="23">
         <v>534</v>
       </c>
-      <c r="I17" s="30">
+      <c r="I17" s="23">
         <v>17</v>
       </c>
-      <c r="J17" s="31">
-        <v>2874</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="J17" s="24">
+        <f t="shared" si="0"/>
+        <v>2891</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="22">
         <v>76</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="22">
         <v>588</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="22">
         <v>1029</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="22">
         <v>196</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="22">
         <v>115</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="23">
         <v>94</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="23">
         <v>6</v>
       </c>
-      <c r="J18" s="31">
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="J18" s="24">
+        <f t="shared" si="0"/>
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="29">
-        <v>0</v>
-      </c>
-      <c r="D19" s="29">
-        <v>0</v>
-      </c>
-      <c r="E19" s="29">
+      <c r="C19" s="22">
+        <v>0</v>
+      </c>
+      <c r="D19" s="22">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22">
         <v>51</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="22">
         <v>879</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="22">
         <v>407</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="23">
         <v>393</v>
       </c>
-      <c r="I19" s="30">
+      <c r="I19" s="23">
         <v>18</v>
       </c>
-      <c r="J19" s="31">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+      <c r="J19" s="24">
+        <f t="shared" si="0"/>
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="29">
-        <v>0</v>
-      </c>
-      <c r="D20" s="29">
-        <v>0</v>
-      </c>
-      <c r="E20" s="29">
-        <v>0</v>
-      </c>
-      <c r="F20" s="29">
+      <c r="C20" s="22">
+        <v>0</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0</v>
+      </c>
+      <c r="F20" s="22">
         <v>112</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="22">
         <v>1163</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="23">
         <v>2111</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="23">
         <v>1574</v>
       </c>
-      <c r="J20" s="31">
-        <v>3386</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="J20" s="24">
+        <f t="shared" si="0"/>
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="29">
-        <v>0</v>
-      </c>
-      <c r="D21" s="29">
-        <v>0</v>
-      </c>
-      <c r="E21" s="29">
-        <v>0</v>
-      </c>
-      <c r="F21" s="29">
+      <c r="C21" s="22">
+        <v>0</v>
+      </c>
+      <c r="D21" s="22">
+        <v>0</v>
+      </c>
+      <c r="E21" s="22">
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
         <v>250</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="22">
         <v>1015</v>
       </c>
-      <c r="H21" s="30">
+      <c r="H21" s="23">
         <v>1728</v>
       </c>
-      <c r="I21" s="30">
+      <c r="I21" s="23">
         <v>2157</v>
       </c>
-      <c r="J21" s="31">
-        <v>2993</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
+      <c r="J21" s="24">
+        <f t="shared" si="0"/>
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="29">
-        <v>0</v>
-      </c>
-      <c r="D22" s="29">
+      <c r="C22" s="22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="22">
         <v>93</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="22">
         <v>569</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="22">
         <v>407</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="22">
         <v>2</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I22" s="23">
         <v>1121</v>
       </c>
-      <c r="J22" s="31">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="28" t="s">
+      <c r="J22" s="24">
+        <f t="shared" si="0"/>
+        <v>2192</v>
+      </c>
+      <c r="L22" s="38"/>
+    </row>
+    <row r="23" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="29">
-        <v>0</v>
-      </c>
-      <c r="D23" s="29">
-        <v>0</v>
-      </c>
-      <c r="E23" s="29">
+      <c r="C23" s="22">
+        <v>0</v>
+      </c>
+      <c r="D23" s="22">
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
         <v>526</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="22">
         <v>449</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="22">
         <v>63</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H23" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="23">
         <v>903</v>
       </c>
-      <c r="J23" s="31">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
+      <c r="J23" s="24">
+        <f t="shared" si="0"/>
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="29">
-        <v>0</v>
-      </c>
-      <c r="D24" s="29">
+      <c r="C24" s="22">
+        <v>0</v>
+      </c>
+      <c r="D24" s="22">
         <v>965</v>
       </c>
-      <c r="E24" s="29">
-        <v>0</v>
-      </c>
-      <c r="F24" s="29">
-        <v>0</v>
-      </c>
-      <c r="G24" s="29">
-        <v>0</v>
-      </c>
-      <c r="H24" s="30">
-        <v>0</v>
-      </c>
-      <c r="I24" s="30">
+      <c r="E24" s="22">
+        <v>0</v>
+      </c>
+      <c r="F24" s="22">
+        <v>0</v>
+      </c>
+      <c r="G24" s="22">
+        <v>0</v>
+      </c>
+      <c r="H24" s="23">
+        <v>0</v>
+      </c>
+      <c r="I24" s="23">
         <v>707</v>
       </c>
-      <c r="J24" s="31">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
+      <c r="J24" s="24">
+        <f t="shared" si="0"/>
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="29">
-        <v>0</v>
-      </c>
-      <c r="D25" s="29">
-        <v>0</v>
-      </c>
-      <c r="E25" s="29">
-        <v>0</v>
-      </c>
-      <c r="F25" s="29">
-        <v>0</v>
-      </c>
-      <c r="G25" s="29">
+      <c r="C25" s="22">
+        <v>0</v>
+      </c>
+      <c r="D25" s="22">
+        <v>0</v>
+      </c>
+      <c r="E25" s="22">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
+        <v>0</v>
+      </c>
+      <c r="G25" s="22">
         <v>892</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="23">
         <v>5995</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="23">
         <v>3772</v>
       </c>
-      <c r="J25" s="31">
-        <v>6887</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="J25" s="24">
+        <f t="shared" si="0"/>
+        <v>10659</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="22">
         <v>310</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="22">
         <v>2</v>
       </c>
-      <c r="E26" s="29">
-        <v>0</v>
-      </c>
-      <c r="F26" s="29">
-        <v>0</v>
-      </c>
-      <c r="G26" s="29">
-        <v>0</v>
-      </c>
-      <c r="H26" s="30" t="s">
+      <c r="E26" s="22">
+        <v>0</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0</v>
+      </c>
+      <c r="G26" s="22">
+        <v>0</v>
+      </c>
+      <c r="H26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="30">
+      <c r="I26" s="23">
         <v>544</v>
       </c>
-      <c r="J26" s="31">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+      <c r="J26" s="24">
+        <f t="shared" si="0"/>
+        <v>856</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="29">
-        <v>0</v>
-      </c>
-      <c r="D27" s="29">
-        <v>0</v>
-      </c>
-      <c r="E27" s="29">
-        <v>0</v>
-      </c>
-      <c r="F27" s="29">
-        <v>0</v>
-      </c>
-      <c r="G27" s="29">
+      <c r="C27" s="22">
+        <v>0</v>
+      </c>
+      <c r="D27" s="22">
+        <v>0</v>
+      </c>
+      <c r="E27" s="22">
+        <v>0</v>
+      </c>
+      <c r="F27" s="22">
+        <v>0</v>
+      </c>
+      <c r="G27" s="22">
         <v>208</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="23">
         <v>18028</v>
       </c>
-      <c r="I27" s="30">
+      <c r="I27" s="23">
         <v>21315</v>
       </c>
-      <c r="J27" s="31">
-        <v>18236</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+      <c r="J27" s="24">
+        <f t="shared" si="0"/>
+        <v>39551</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="29">
-        <v>0</v>
-      </c>
-      <c r="D28" s="29">
-        <v>0</v>
-      </c>
-      <c r="E28" s="29">
-        <v>0</v>
-      </c>
-      <c r="F28" s="29">
-        <v>0</v>
-      </c>
-      <c r="G28" s="29">
+      <c r="C28" s="22">
+        <v>0</v>
+      </c>
+      <c r="D28" s="22">
+        <v>0</v>
+      </c>
+      <c r="E28" s="22">
+        <v>0</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0</v>
+      </c>
+      <c r="G28" s="22">
         <v>118</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="23">
         <v>550</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I28" s="23">
         <v>666</v>
       </c>
-      <c r="J28" s="31">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="32" t="s">
+      <c r="J28" s="24">
+        <f t="shared" si="0"/>
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="33">
-        <v>0</v>
-      </c>
-      <c r="D29" s="33">
-        <v>0</v>
-      </c>
-      <c r="E29" s="33">
-        <v>0</v>
-      </c>
-      <c r="F29" s="33">
-        <v>0</v>
-      </c>
-      <c r="G29" s="33">
+      <c r="C29" s="26">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26">
+        <v>0</v>
+      </c>
+      <c r="F29" s="26">
+        <v>0</v>
+      </c>
+      <c r="G29" s="26">
         <v>86</v>
       </c>
-      <c r="H29" s="34">
+      <c r="H29" s="27">
         <v>2020</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="27">
         <v>531</v>
       </c>
-      <c r="J29" s="31">
-        <v>2106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
+      <c r="J29" s="24">
+        <f t="shared" si="0"/>
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="29">
+      <c r="B30" s="30"/>
+      <c r="C30" s="22">
+        <f>SUM(C2:C29)</f>
         <v>17731</v>
       </c>
-      <c r="D30" s="29">
-        <v>48200</v>
-      </c>
-      <c r="E30" s="29">
+      <c r="D30" s="22">
+        <f t="shared" ref="D30:I30" si="1">SUM(D2:D29)</f>
+        <v>53234</v>
+      </c>
+      <c r="E30" s="22">
+        <f t="shared" si="1"/>
         <v>96702</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="22">
+        <f t="shared" si="1"/>
         <v>118773</v>
       </c>
-      <c r="G30" s="29">
-        <v>113869</v>
-      </c>
-      <c r="H30" s="29">
+      <c r="G30" s="22">
+        <f t="shared" si="1"/>
+        <v>115079</v>
+      </c>
+      <c r="H30" s="22">
+        <f t="shared" si="1"/>
         <v>144035</v>
       </c>
-      <c r="I30" s="29">
-        <f>SUM(I2:I29)</f>
+      <c r="I30" s="22">
+        <f t="shared" si="1"/>
         <v>149484</v>
       </c>
-      <c r="J30" s="31">
-        <v>539310</v>
+      <c r="J30" s="24">
+        <f>SUM(C30:I30)</f>
+        <v>695038</v>
       </c>
     </row>
     <row r="33" spans="2:56" s="1" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
@@ -2544,18 +2586,18 @@
       <c r="BD33" s="4"/>
     </row>
     <row r="34" spans="2:56" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
@@ -2591,18 +2633,18 @@
       <c r="BD34" s="5"/>
     </row>
     <row r="35" spans="2:56" s="1" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
       <c r="L35" s="7"/>
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
@@ -2638,18 +2680,18 @@
       <c r="BD35" s="5"/>
     </row>
     <row r="36" spans="2:56" s="1" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
       <c r="N36" s="7"/>
@@ -2685,18 +2727,18 @@
       <c r="BD36" s="5"/>
     </row>
     <row r="37" spans="2:56" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
@@ -2717,18 +2759,18 @@
       <c r="AI37" s="2"/>
     </row>
     <row r="38" spans="2:56" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
@@ -2749,18 +2791,18 @@
       <c r="AI38" s="2"/>
     </row>
     <row r="39" spans="2:56" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
@@ -2781,18 +2823,18 @@
       <c r="AI39" s="2"/>
     </row>
     <row r="40" spans="2:56" s="1" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7"/>
       <c r="N40" s="7"/>
@@ -2869,33 +2911,33 @@
   <sheetData>
     <row r="1" spans="2:31" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
     </row>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">

</xml_diff>